<commit_message>
finish forward rate swap
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\GR6250-2019\hw8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Shen\Source\Repos\hw8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AA1B6-3A3A-449C-8E4D-534C3B62A88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A7AE68-300F-4825-88DE-2B6D1F5B7C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +43,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Create handles to fra's and swaps</t>
         </r>
@@ -57,14 +54,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -133,25 +130,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +157,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -297,7 +301,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1020,7 +1024,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="492912992"/>
@@ -1082,7 +1086,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="492912664"/>
@@ -1130,7 +1134,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2038,17 +2042,20 @@
   <dimension ref="B2:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2057,10 +2064,10 @@
       </c>
       <c r="I4" cm="1">
         <f t="array" ref="I4">_xll.PWFLAT.FORWARD(C5:C17,E5:E17)</f>
-        <v>-1887632</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2073,7 +2080,7 @@
       </c>
       <c r="F5" cm="1">
         <f t="array" ref="F5">_xll.INSTRUMENT.CASH_DEPOSIT(C5, E5)</f>
-        <v>276992</v>
+        <v>-256</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2083,7 +2090,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2096,7 +2103,7 @@
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">_xll.INSTRUMENT.CASH_DEPOSIT(C6, E6)</f>
-        <v>276680</v>
+        <v>-168</v>
       </c>
       <c r="H6">
         <v>0.1</v>
@@ -2105,7 +2112,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2118,7 +2125,7 @@
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">_xll.INSTRUMENT.CASH_DEPOSIT(C7, E7)</f>
-        <v>276776</v>
+        <v>-278</v>
       </c>
       <c r="H7">
         <v>0.2</v>
@@ -2127,7 +2134,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2140,7 +2147,7 @@
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.INSTRUMENT.CASH_DEPOSIT(C8, E8)</f>
-        <v>276728</v>
+        <v>-124</v>
       </c>
       <c r="H8">
         <v>0.3</v>
@@ -2149,7 +2156,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2162,7 +2169,7 @@
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">_xll.INSTRUMENT.CASH_DEPOSIT(C9, E9)</f>
-        <v>276704</v>
+        <v>8</v>
       </c>
       <c r="H9">
         <v>0.4</v>
@@ -2171,7 +2178,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2191,10 @@
       <c r="E10">
         <v>0.02</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,E10)</f>
+        <v>-212</v>
+      </c>
       <c r="H10">
         <v>0.5</v>
       </c>
@@ -2192,7 +2202,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2215,10 @@
       <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,E11)</f>
+        <v>-476</v>
+      </c>
       <c r="H11">
         <v>0.6</v>
       </c>
@@ -2213,7 +2226,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2239,10 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,E12)</f>
+        <v>-454</v>
+      </c>
       <c r="H12">
         <v>0.7</v>
       </c>
@@ -2234,7 +2250,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2263,10 @@
       <c r="E13">
         <v>0.02</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,E13)</f>
+        <v>-432</v>
+      </c>
       <c r="H13">
         <v>0.8</v>
       </c>
@@ -2255,7 +2274,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2287,10 @@
       <c r="E14">
         <v>0.03</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
+        <v>12462044</v>
+      </c>
       <c r="H14">
         <v>0.9</v>
       </c>
@@ -2276,7 +2298,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2311,10 @@
       <c r="E15">
         <v>0.03</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
+        <v>-322</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
@@ -2297,7 +2322,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +2335,10 @@
       <c r="E16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
+        <v>-344</v>
+      </c>
       <c r="H16">
         <v>1.1000000000000001</v>
       </c>
@@ -2318,7 +2346,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2359,10 @@
       <c r="E17">
         <v>0.03</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
+        <v>-300</v>
+      </c>
       <c r="H17">
         <v>1.2</v>
       </c>
@@ -2339,7 +2370,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H18">
         <v>1.3</v>
       </c>
@@ -2347,7 +2378,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H19">
         <v>1.4</v>
       </c>
@@ -2355,7 +2386,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H20">
         <v>1.5</v>
       </c>
@@ -2363,7 +2394,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H21">
         <v>1.6</v>
       </c>
@@ -2371,7 +2402,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H22">
         <v>1.7</v>
       </c>
@@ -2379,7 +2410,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H23">
         <v>1.8</v>
       </c>
@@ -2387,7 +2418,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H24">
         <v>1.9</v>
       </c>
@@ -2395,7 +2426,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H25">
         <v>2</v>
       </c>
@@ -2403,7 +2434,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H26">
         <v>2.1</v>
       </c>
@@ -2411,7 +2442,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
@@ -2419,7 +2450,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
@@ -2427,7 +2458,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H29">
         <v>2.4</v>
       </c>
@@ -2435,7 +2466,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H30">
         <v>2.5</v>
       </c>
@@ -2443,7 +2474,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H31">
         <v>2.6</v>
       </c>
@@ -2451,7 +2482,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H32">
         <v>2.7</v>
       </c>
@@ -2459,7 +2490,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H33">
         <v>2.8</v>
       </c>
@@ -2467,7 +2498,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H34">
         <v>2.9</v>
       </c>
@@ -2475,7 +2506,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H35">
         <v>3</v>
       </c>
@@ -2483,7 +2514,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H36">
         <v>3.1</v>
       </c>
@@ -2491,7 +2522,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H37">
         <v>3.2</v>
       </c>
@@ -2499,7 +2530,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H38">
         <v>3.3</v>
       </c>
@@ -2507,7 +2538,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H39">
         <v>3.4</v>
       </c>
@@ -2515,7 +2546,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H40">
         <v>3.5</v>
       </c>
@@ -2523,7 +2554,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H41">
         <v>3.6</v>
       </c>
@@ -2531,7 +2562,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H42">
         <v>3.7</v>
       </c>
@@ -2539,7 +2570,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H43">
         <v>3.8</v>
       </c>
@@ -2547,7 +2578,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H44">
         <v>3.9</v>
       </c>
@@ -2555,7 +2586,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H45">
         <v>4</v>
       </c>
@@ -2563,7 +2594,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
@@ -2571,7 +2602,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H47">
         <v>4.2</v>
       </c>
@@ -2579,7 +2610,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H48">
         <v>4.3</v>
       </c>
@@ -2587,7 +2618,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
@@ -2595,7 +2626,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H50">
         <v>4.5</v>
       </c>
@@ -2603,7 +2634,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
@@ -2611,7 +2642,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H52">
         <v>4.7</v>
       </c>
@@ -2619,7 +2650,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H53">
         <v>4.8</v>
       </c>
@@ -2627,7 +2658,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
@@ -2635,7 +2666,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H55">
         <v>5</v>
       </c>
@@ -2643,7 +2674,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
@@ -2651,7 +2682,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H57">
         <v>5.2</v>
       </c>
@@ -2659,7 +2690,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H58">
         <v>5.3</v>
       </c>
@@ -2667,7 +2698,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H59">
         <v>5.4</v>
       </c>
@@ -2675,7 +2706,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H60">
         <v>5.5</v>
       </c>
@@ -2683,7 +2714,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H61">
         <v>5.6</v>
       </c>
@@ -2691,7 +2722,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H62">
         <v>5.7</v>
       </c>
@@ -2699,7 +2730,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H63">
         <v>5.8</v>
       </c>
@@ -2707,7 +2738,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H64">
         <v>5.9</v>
       </c>
@@ -2715,7 +2746,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H65">
         <v>6</v>
       </c>
@@ -2723,7 +2754,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H66">
         <v>6.1</v>
       </c>
@@ -2731,7 +2762,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H67">
         <v>6.2</v>
       </c>
@@ -2739,7 +2770,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H68">
         <v>6.3</v>
       </c>
@@ -2747,7 +2778,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H69">
         <v>6.4</v>
       </c>
@@ -2755,7 +2786,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H70">
         <v>6.5</v>
       </c>
@@ -2763,7 +2794,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H71">
         <v>6.6</v>
       </c>
@@ -2771,7 +2802,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H72">
         <v>6.7</v>
       </c>
@@ -2779,7 +2810,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H73">
         <v>6.8</v>
       </c>
@@ -2787,7 +2818,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H74">
         <v>6.9</v>
       </c>
@@ -2795,7 +2826,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H75">
         <v>7</v>
       </c>
@@ -2803,7 +2834,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H76">
         <v>7.1</v>
       </c>
@@ -2811,7 +2842,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H77">
         <v>7.2</v>
       </c>
@@ -2819,7 +2850,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H78">
         <v>7.3</v>
       </c>
@@ -2827,7 +2858,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H79">
         <v>7.4</v>
       </c>
@@ -2835,7 +2866,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H80">
         <v>7.5</v>
       </c>
@@ -2843,7 +2874,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H81">
         <v>7.6</v>
       </c>
@@ -2851,7 +2882,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H82">
         <v>7.7</v>
       </c>
@@ -2859,7 +2890,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H83">
         <v>7.8</v>
       </c>
@@ -2867,7 +2898,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H84">
         <v>7.9</v>
       </c>
@@ -2875,7 +2906,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H85">
         <v>8</v>
       </c>
@@ -2883,7 +2914,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H86">
         <v>8.1</v>
       </c>
@@ -2891,7 +2922,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
@@ -2899,7 +2930,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
@@ -2907,7 +2938,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H89">
         <v>8.4</v>
       </c>
@@ -2915,7 +2946,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H90">
         <v>8.5</v>
       </c>
@@ -2923,7 +2954,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H91">
         <v>8.6</v>
       </c>
@@ -2931,7 +2962,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
@@ -2939,7 +2970,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
@@ -2947,7 +2978,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H94">
         <v>8.9</v>
       </c>
@@ -2955,7 +2986,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H95">
         <v>9</v>
       </c>
@@ -2963,7 +2994,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H96">
         <v>9.1</v>
       </c>
@@ -2971,7 +3002,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
@@ -2979,7 +3010,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
@@ -2987,7 +3018,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
@@ -2995,7 +3026,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H100">
         <v>9.5</v>
       </c>
@@ -3003,7 +3034,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H101">
         <v>9.6</v>
       </c>
@@ -3011,7 +3042,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
@@ -3019,7 +3050,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
@@ -3027,7 +3058,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
@@ -3035,7 +3066,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H105">
         <v>10</v>
       </c>
@@ -3044,6 +3075,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
complete spot and discount
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Shen\Source\Repos\hw8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A7AE68-300F-4825-88DE-2B6D1F5B7C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A64A9E9-5383-4073-AB97-C8B98E23E0A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -284,26 +285,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -312,8 +293,645 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$5:$H$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$5:$I$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-72C4-4787-90F5-0982F014F2CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -953,7 +1571,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C739-4CD9-A51E-EB38AAA39F5E}"/>
+              <c16:uniqueId val="{00000001-72C4-4787-90F5-0982F014F2CE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1093,40 +1711,12 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -1145,576 +1735,1724 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Discount</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$5:$H$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$J$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99900049983337502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99800199866733308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.997004495503373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99600798934399148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99501247919268232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99401796405393528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99302444293323511</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99203191483706066</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99104037877288365</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99004983374916811</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98807171286193052</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98609754426286189</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98412732005528514</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98216103235830077</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98019867330675525</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.97824023505121005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97628570975790929</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.97433508960874937</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.97238836680124685</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97044553354850815</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.96753855958903201</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96464029348312308</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.96175070914636673</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.95886978057248451</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.95599748183309996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.95313378707750473</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.95027867053242698</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.94743210650179832</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.94459406936652335</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.94176453358424872</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.93894347368913322</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93613086429161885</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.93332668007820196</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93053089581120574</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.92774348632855286</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.92496442654353928</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.92219369144460805</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.91943125609512466</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.91667709563315225</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.91393118527122819</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.91119350029614055</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.90846401606870619</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9057427080235485</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.90302955166887677</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.90032452258626561</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.89762759643043488</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.89493874892903102</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.8922579558824083</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.88958519316341134</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.88692043671715748</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.8842636625608209</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.88161484678341606</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.87897396554558316</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.87634099507937324</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.87371591168803442</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.87109869174579835</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.86848931169766785</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.86588774805920499</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.86329397741631941</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.86070797642505781</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.8581297218113938</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.85555919037101846</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.85299635896913151</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.85044120454023298</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.84789370408791587</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.84535383468465874</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.8428215734716199</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.84029689765843141</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.83777978452299384</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.835270211411272</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.83276815573709095</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.83027359498193265</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.82778650669473364</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.82530686849168233</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.82283465805601841</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.82036985313783106</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.8179124315538594</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.8154623711872927</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.81301964998757104</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.81058424597018708</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.80815613721648838</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.80573530187347964</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.80332171815362652</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.80091536433465915</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.79851621875937706</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.79612425983545376</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.79373946603524281</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.79136181589558385</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.78899128801760976</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.78662786106655347</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.78427151377155646</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.78192222492547725</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.77957997338470042</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.7772447380689459</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.77491649796108097</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.77259523210692804</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.77028091961507894</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.76797353965670601</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.76567307146537378</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.76337949433685315</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-34F0-4EB3-A793-C36F1CE3EEE0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="492912664"/>
+        <c:axId val="492912992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="492912664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492912992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="492912992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492912664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Spot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
         <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$5:$H$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$5:$K$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999996966E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999395E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999187E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.999999999999969E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9999999999999863E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9999999999999811E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999967E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999655E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9999999999999464E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0909090909090929E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1666666666666678E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2307692307692289E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2857142857142822E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3333333333333365E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3749999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4117647058823542E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4444444444444418E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.473684210526318E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5000000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.6363636363636341E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6956521739130429E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7500000000000019E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.8461538461538463E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8888888888888868E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.9285714285714278E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.9655172413793106E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.9999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.0322580645161296E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.0625000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.0909090909090908E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.1176470588235293E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.1428571428571439E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.1666666666666667E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.1891891891891894E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.2105263157894742E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.230769230769232E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.2499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.2682926829268299E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.2857142857142843E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.3023255813953487E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.3181818181818192E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.3333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.3478260869565219E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.3617021276595738E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.3750000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.3877551020408162E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.4000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.4117647058823525E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.4230769230769226E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.4339622641509441E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.4444444444444453E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.4545454545454547E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.4642857142857147E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.4736842105263165E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.4827586206896561E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.4915254237288138E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.5081967213114755E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.5161290322580646E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.523809523809524E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.5312500000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.5384615384615377E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.5454545454545452E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.5522388059701497E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.5588235294117655E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.5652173913043478E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.5714285714285717E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5774647887323945E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.583333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.5890410958904111E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.5945945945945952E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.6052631578947362E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.6103896103896105E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.6153846153846149E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.6202531645569613E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.6250000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.6296296296296297E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.6341463414634152E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.6385542168674697E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.642857142857143E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.6470588235294114E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.651162790697674E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.655172413793103E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.6590909090909089E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.662921348314606E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.6666666666666658E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.6703296703296703E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.6739130434782613E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.6774193548387091E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.6808510638297881E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.6842105263157889E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.6875000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.6907216494845364E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.6938775510204079E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.6969696969696963E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.7000000000000007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B6A6-456C-84FD-A4771B1CFA9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="492912664"/>
+        <c:axId val="492912992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="492912664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492912992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="492912992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492912664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>88106</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>54768</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>69056</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>150018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>126206</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>83343</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>107156</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>178593</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1734,6 +3472,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{372761CA-D993-4A23-AABC-9CB0A9457A06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0685B06-7690-462F-8095-EAB5F086AB87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2039,10 +3853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E377A32-36B0-46CA-9461-D5EEF7A10455}">
-  <dimension ref="B2:I105"/>
+  <dimension ref="B2:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2050,12 +3864,12 @@
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2067,7 +3881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2080,7 +3894,7 @@
       </c>
       <c r="F5" cm="1">
         <f t="array" ref="F5">_xll.INSTRUMENT.CASH_DEPOSIT(C5, E5)</f>
-        <v>-256</v>
+        <v>-344</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2089,8 +3903,16 @@
         <f t="array" ref="I5:I105">_xll.PWFLAT.FORWARD.VALUE(I4,H5:H105)</f>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <f t="array" ref="J5:J105">_xll.PWFLAT.FORWARD.DISCOUNT(I4,H5:H105)</f>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="array" ref="K5:K105">_xll.PWFLAT.FORWARD.SPOT(I4,H5:H105)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2103,7 +3925,7 @@
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">_xll.INSTRUMENT.CASH_DEPOSIT(C6, E6)</f>
-        <v>-168</v>
+        <v>-190</v>
       </c>
       <c r="H6">
         <v>0.1</v>
@@ -2111,8 +3933,14 @@
       <c r="I6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0.99900049983337502</v>
+      </c>
+      <c r="K6">
+        <v>9.9999999999996966E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2125,7 +3953,7 @@
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">_xll.INSTRUMENT.CASH_DEPOSIT(C7, E7)</f>
-        <v>-278</v>
+        <v>-256</v>
       </c>
       <c r="H7">
         <v>0.2</v>
@@ -2133,8 +3961,14 @@
       <c r="I7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0.99800199866733308</v>
+      </c>
+      <c r="K7">
+        <v>9.9999999999999395E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2147,7 +3981,7 @@
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.INSTRUMENT.CASH_DEPOSIT(C8, E8)</f>
-        <v>-124</v>
+        <v>-278</v>
       </c>
       <c r="H8">
         <v>0.3</v>
@@ -2155,8 +3989,14 @@
       <c r="I8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0.997004495503373</v>
+      </c>
+      <c r="K8">
+        <v>9.9999999999999187E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2169,7 +4009,7 @@
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">_xll.INSTRUMENT.CASH_DEPOSIT(C9, E9)</f>
-        <v>8</v>
+        <v>-168</v>
       </c>
       <c r="H9">
         <v>0.4</v>
@@ -2177,8 +4017,14 @@
       <c r="I9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>0.99600798934399148</v>
+      </c>
+      <c r="K9">
+        <v>9.999999999999969E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2193,7 +4039,7 @@
       </c>
       <c r="F10" s="4">
         <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,E10)</f>
-        <v>-212</v>
+        <v>-36</v>
       </c>
       <c r="H10">
         <v>0.5</v>
@@ -2201,8 +4047,14 @@
       <c r="I10">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>0.99501247919268232</v>
+      </c>
+      <c r="K10">
+        <v>9.9999999999999863E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2217,7 +4069,7 @@
       </c>
       <c r="F11" s="4">
         <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,E11)</f>
-        <v>-476</v>
+        <v>-124</v>
       </c>
       <c r="H11">
         <v>0.6</v>
@@ -2225,8 +4077,14 @@
       <c r="I11">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.99401796405393528</v>
+      </c>
+      <c r="K11">
+        <v>9.9999999999999811E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2241,7 +4099,7 @@
       </c>
       <c r="F12" s="4">
         <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,E12)</f>
-        <v>-454</v>
+        <v>-234</v>
       </c>
       <c r="H12">
         <v>0.7</v>
@@ -2249,8 +4107,14 @@
       <c r="I12">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.99302444293323511</v>
+      </c>
+      <c r="K12">
+        <v>9.9999999999999967E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2265,7 +4129,7 @@
       </c>
       <c r="F13" s="4">
         <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,E13)</f>
-        <v>-432</v>
+        <v>-322</v>
       </c>
       <c r="H13">
         <v>0.8</v>
@@ -2273,8 +4137,14 @@
       <c r="I13">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0.99203191483706066</v>
+      </c>
+      <c r="K13">
+        <v>9.9999999999999655E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2289,7 +4159,7 @@
       </c>
       <c r="F14" s="4">
         <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
-        <v>12462044</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <v>0.9</v>
@@ -2297,8 +4167,14 @@
       <c r="I14">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>0.99104037877288365</v>
+      </c>
+      <c r="K14">
+        <v>1.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2313,7 +4189,7 @@
       </c>
       <c r="F15" s="4">
         <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
-        <v>-322</v>
+        <v>-212</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2321,8 +4197,14 @@
       <c r="I15">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>0.99004983374916811</v>
+      </c>
+      <c r="K15">
+        <v>9.9999999999999464E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2337,7 +4219,7 @@
       </c>
       <c r="F16" s="4">
         <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
-        <v>-344</v>
+        <v>-300</v>
       </c>
       <c r="H16">
         <v>1.1000000000000001</v>
@@ -2345,8 +4227,14 @@
       <c r="I16">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>0.98807171286193052</v>
+      </c>
+      <c r="K16">
+        <v>1.0909090909090929E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2361,7 +4249,7 @@
       </c>
       <c r="F17" s="4">
         <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
-        <v>-300</v>
+        <v>-102</v>
       </c>
       <c r="H17">
         <v>1.2</v>
@@ -2369,709 +4257,1243 @@
       <c r="I17">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>0.98609754426286189</v>
+      </c>
+      <c r="K17">
+        <v>1.1666666666666678E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H18">
         <v>1.3</v>
       </c>
       <c r="I18">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>0.98412732005528514</v>
+      </c>
+      <c r="K18">
+        <v>1.2307692307692289E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H19">
         <v>1.4</v>
       </c>
       <c r="I19">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>0.98216103235830077</v>
+      </c>
+      <c r="K19">
+        <v>1.2857142857142822E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H20">
         <v>1.5</v>
       </c>
       <c r="I20">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>0.98019867330675525</v>
+      </c>
+      <c r="K20">
+        <v>1.3333333333333365E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H21">
         <v>1.6</v>
       </c>
       <c r="I21">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>0.97824023505121005</v>
+      </c>
+      <c r="K21">
+        <v>1.3749999999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H22">
         <v>1.7</v>
       </c>
       <c r="I22">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>0.97628570975790929</v>
+      </c>
+      <c r="K22">
+        <v>1.4117647058823542E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H23">
         <v>1.8</v>
       </c>
       <c r="I23">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>0.97433508960874937</v>
+      </c>
+      <c r="K23">
+        <v>1.4444444444444418E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H24">
         <v>1.9</v>
       </c>
       <c r="I24">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>0.97238836680124685</v>
+      </c>
+      <c r="K24">
+        <v>1.473684210526318E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H25">
         <v>2</v>
       </c>
       <c r="I25">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>0.97044553354850815</v>
+      </c>
+      <c r="K25">
+        <v>1.5000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H26">
         <v>2.1</v>
       </c>
       <c r="I26">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>0.96753855958903201</v>
+      </c>
+      <c r="K26">
+        <v>1.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
       <c r="I27">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>0.96464029348312308</v>
+      </c>
+      <c r="K27">
+        <v>1.6363636363636341E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
       <c r="I28">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>0.96175070914636673</v>
+      </c>
+      <c r="K28">
+        <v>1.6956521739130429E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H29">
         <v>2.4</v>
       </c>
       <c r="I29">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>0.95886978057248451</v>
+      </c>
+      <c r="K29">
+        <v>1.7500000000000019E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H30">
         <v>2.5</v>
       </c>
       <c r="I30">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>0.95599748183309996</v>
+      </c>
+      <c r="K30">
+        <v>1.7999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H31">
         <v>2.6</v>
       </c>
       <c r="I31">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>0.95313378707750473</v>
+      </c>
+      <c r="K31">
+        <v>1.8461538461538463E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H32">
         <v>2.7</v>
       </c>
       <c r="I32">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>0.95027867053242698</v>
+      </c>
+      <c r="K32">
+        <v>1.8888888888888868E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H33">
         <v>2.8</v>
       </c>
       <c r="I33">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>0.94743210650179832</v>
+      </c>
+      <c r="K33">
+        <v>1.9285714285714278E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H34">
         <v>2.9</v>
       </c>
       <c r="I34">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>0.94459406936652335</v>
+      </c>
+      <c r="K34">
+        <v>1.9655172413793106E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H35">
         <v>3</v>
       </c>
       <c r="I35">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>0.94176453358424872</v>
+      </c>
+      <c r="K35">
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H36">
         <v>3.1</v>
       </c>
       <c r="I36">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>0.93894347368913322</v>
+      </c>
+      <c r="K36">
+        <v>2.0322580645161296E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H37">
         <v>3.2</v>
       </c>
       <c r="I37">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>0.93613086429161885</v>
+      </c>
+      <c r="K37">
+        <v>2.0625000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H38">
         <v>3.3</v>
       </c>
       <c r="I38">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>0.93332668007820196</v>
+      </c>
+      <c r="K38">
+        <v>2.0909090909090908E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H39">
         <v>3.4</v>
       </c>
       <c r="I39">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>0.93053089581120574</v>
+      </c>
+      <c r="K39">
+        <v>2.1176470588235293E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H40">
         <v>3.5</v>
       </c>
       <c r="I40">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>0.92774348632855286</v>
+      </c>
+      <c r="K40">
+        <v>2.1428571428571439E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H41">
         <v>3.6</v>
       </c>
       <c r="I41">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>0.92496442654353928</v>
+      </c>
+      <c r="K41">
+        <v>2.1666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H42">
         <v>3.7</v>
       </c>
       <c r="I42">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>0.92219369144460805</v>
+      </c>
+      <c r="K42">
+        <v>2.1891891891891894E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H43">
         <v>3.8</v>
       </c>
       <c r="I43">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>0.91943125609512466</v>
+      </c>
+      <c r="K43">
+        <v>2.2105263157894742E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H44">
         <v>3.9</v>
       </c>
       <c r="I44">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>0.91667709563315225</v>
+      </c>
+      <c r="K44">
+        <v>2.230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H45">
         <v>4</v>
       </c>
       <c r="I45">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>0.91393118527122819</v>
+      </c>
+      <c r="K45">
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
       <c r="I46">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>0.91119350029614055</v>
+      </c>
+      <c r="K46">
+        <v>2.2682926829268299E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H47">
         <v>4.2</v>
       </c>
       <c r="I47">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>0.90846401606870619</v>
+      </c>
+      <c r="K47">
+        <v>2.2857142857142843E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H48">
         <v>4.3</v>
       </c>
       <c r="I48">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>0.9057427080235485</v>
+      </c>
+      <c r="K48">
+        <v>2.3023255813953487E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
       <c r="I49">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>0.90302955166887677</v>
+      </c>
+      <c r="K49">
+        <v>2.3181818181818192E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H50">
         <v>4.5</v>
       </c>
       <c r="I50">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>0.90032452258626561</v>
+      </c>
+      <c r="K50">
+        <v>2.3333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
       <c r="I51">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>0.89762759643043488</v>
+      </c>
+      <c r="K51">
+        <v>2.3478260869565219E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H52">
         <v>4.7</v>
       </c>
       <c r="I52">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>0.89493874892903102</v>
+      </c>
+      <c r="K52">
+        <v>2.3617021276595738E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H53">
         <v>4.8</v>
       </c>
       <c r="I53">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>0.8922579558824083</v>
+      </c>
+      <c r="K53">
+        <v>2.3750000000000004E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
       <c r="I54">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>0.88958519316341134</v>
+      </c>
+      <c r="K54">
+        <v>2.3877551020408162E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H55">
         <v>5</v>
       </c>
       <c r="I55">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>0.88692043671715748</v>
+      </c>
+      <c r="K55">
+        <v>2.4000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
       <c r="I56">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>0.8842636625608209</v>
+      </c>
+      <c r="K56">
+        <v>2.4117647058823525E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H57">
         <v>5.2</v>
       </c>
       <c r="I57">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>0.88161484678341606</v>
+      </c>
+      <c r="K57">
+        <v>2.4230769230769226E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H58">
         <v>5.3</v>
       </c>
       <c r="I58">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>0.87897396554558316</v>
+      </c>
+      <c r="K58">
+        <v>2.4339622641509441E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H59">
         <v>5.4</v>
       </c>
       <c r="I59">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>0.87634099507937324</v>
+      </c>
+      <c r="K59">
+        <v>2.4444444444444453E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H60">
         <v>5.5</v>
       </c>
       <c r="I60">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>0.87371591168803442</v>
+      </c>
+      <c r="K60">
+        <v>2.4545454545454547E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H61">
         <v>5.6</v>
       </c>
       <c r="I61">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>0.87109869174579835</v>
+      </c>
+      <c r="K61">
+        <v>2.4642857142857147E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H62">
         <v>5.7</v>
       </c>
       <c r="I62">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>0.86848931169766785</v>
+      </c>
+      <c r="K62">
+        <v>2.4736842105263165E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H63">
         <v>5.8</v>
       </c>
       <c r="I63">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J63">
+        <v>0.86588774805920499</v>
+      </c>
+      <c r="K63">
+        <v>2.4827586206896561E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H64">
         <v>5.9</v>
       </c>
       <c r="I64">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>0.86329397741631941</v>
+      </c>
+      <c r="K64">
+        <v>2.4915254237288138E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H65">
         <v>6</v>
       </c>
       <c r="I65">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>0.86070797642505781</v>
+      </c>
+      <c r="K65">
+        <v>2.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H66">
         <v>6.1</v>
       </c>
       <c r="I66">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>0.8581297218113938</v>
+      </c>
+      <c r="K66">
+        <v>2.5081967213114755E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H67">
         <v>6.2</v>
       </c>
       <c r="I67">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J67">
+        <v>0.85555919037101846</v>
+      </c>
+      <c r="K67">
+        <v>2.5161290322580646E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H68">
         <v>6.3</v>
       </c>
       <c r="I68">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>0.85299635896913151</v>
+      </c>
+      <c r="K68">
+        <v>2.523809523809524E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H69">
         <v>6.4</v>
       </c>
       <c r="I69">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J69">
+        <v>0.85044120454023298</v>
+      </c>
+      <c r="K69">
+        <v>2.5312500000000005E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H70">
         <v>6.5</v>
       </c>
       <c r="I70">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>0.84789370408791587</v>
+      </c>
+      <c r="K70">
+        <v>2.5384615384615377E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H71">
         <v>6.6</v>
       </c>
       <c r="I71">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>0.84535383468465874</v>
+      </c>
+      <c r="K71">
+        <v>2.5454545454545452E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H72">
         <v>6.7</v>
       </c>
       <c r="I72">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J72">
+        <v>0.8428215734716199</v>
+      </c>
+      <c r="K72">
+        <v>2.5522388059701497E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H73">
         <v>6.8</v>
       </c>
       <c r="I73">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J73">
+        <v>0.84029689765843141</v>
+      </c>
+      <c r="K73">
+        <v>2.5588235294117655E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H74">
         <v>6.9</v>
       </c>
       <c r="I74">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <v>0.83777978452299384</v>
+      </c>
+      <c r="K74">
+        <v>2.5652173913043478E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H75">
         <v>7</v>
       </c>
       <c r="I75">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J75">
+        <v>0.835270211411272</v>
+      </c>
+      <c r="K75">
+        <v>2.5714285714285717E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H76">
         <v>7.1</v>
       </c>
       <c r="I76">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J76">
+        <v>0.83276815573709095</v>
+      </c>
+      <c r="K76">
+        <v>2.5774647887323945E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H77">
         <v>7.2</v>
       </c>
       <c r="I77">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J77">
+        <v>0.83027359498193265</v>
+      </c>
+      <c r="K77">
+        <v>2.583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H78">
         <v>7.3</v>
       </c>
       <c r="I78">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J78">
+        <v>0.82778650669473364</v>
+      </c>
+      <c r="K78">
+        <v>2.5890410958904111E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H79">
         <v>7.4</v>
       </c>
       <c r="I79">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J79">
+        <v>0.82530686849168233</v>
+      </c>
+      <c r="K79">
+        <v>2.5945945945945952E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H80">
         <v>7.5</v>
       </c>
       <c r="I80">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>0.82283465805601841</v>
+      </c>
+      <c r="K80">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H81">
         <v>7.6</v>
       </c>
       <c r="I81">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J81">
+        <v>0.82036985313783106</v>
+      </c>
+      <c r="K81">
+        <v>2.6052631578947362E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H82">
         <v>7.7</v>
       </c>
       <c r="I82">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J82">
+        <v>0.8179124315538594</v>
+      </c>
+      <c r="K82">
+        <v>2.6103896103896105E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H83">
         <v>7.8</v>
       </c>
       <c r="I83">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J83">
+        <v>0.8154623711872927</v>
+      </c>
+      <c r="K83">
+        <v>2.6153846153846149E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H84">
         <v>7.9</v>
       </c>
       <c r="I84">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J84">
+        <v>0.81301964998757104</v>
+      </c>
+      <c r="K84">
+        <v>2.6202531645569613E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H85">
         <v>8</v>
       </c>
       <c r="I85">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J85">
+        <v>0.81058424597018708</v>
+      </c>
+      <c r="K85">
+        <v>2.6250000000000002E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H86">
         <v>8.1</v>
       </c>
       <c r="I86">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J86">
+        <v>0.80815613721648838</v>
+      </c>
+      <c r="K86">
+        <v>2.6296296296296297E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
       <c r="I87">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>0.80573530187347964</v>
+      </c>
+      <c r="K87">
+        <v>2.6341463414634152E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
       <c r="I88">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>0.80332171815362652</v>
+      </c>
+      <c r="K88">
+        <v>2.6385542168674697E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H89">
         <v>8.4</v>
       </c>
       <c r="I89">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>0.80091536433465915</v>
+      </c>
+      <c r="K89">
+        <v>2.642857142857143E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H90">
         <v>8.5</v>
       </c>
       <c r="I90">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J90">
+        <v>0.79851621875937706</v>
+      </c>
+      <c r="K90">
+        <v>2.6470588235294114E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H91">
         <v>8.6</v>
       </c>
       <c r="I91">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J91">
+        <v>0.79612425983545376</v>
+      </c>
+      <c r="K91">
+        <v>2.651162790697674E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
       <c r="I92">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J92">
+        <v>0.79373946603524281</v>
+      </c>
+      <c r="K92">
+        <v>2.655172413793103E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
       <c r="I93">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J93">
+        <v>0.79136181589558385</v>
+      </c>
+      <c r="K93">
+        <v>2.6590909090909089E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H94">
         <v>8.9</v>
       </c>
       <c r="I94">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>0.78899128801760976</v>
+      </c>
+      <c r="K94">
+        <v>2.662921348314606E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H95">
         <v>9</v>
       </c>
       <c r="I95">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J95">
+        <v>0.78662786106655347</v>
+      </c>
+      <c r="K95">
+        <v>2.6666666666666658E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H96">
         <v>9.1</v>
       </c>
       <c r="I96">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J96">
+        <v>0.78427151377155646</v>
+      </c>
+      <c r="K96">
+        <v>2.6703296703296703E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
       <c r="I97">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J97">
+        <v>0.78192222492547725</v>
+      </c>
+      <c r="K97">
+        <v>2.6739130434782613E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
       <c r="I98">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J98">
+        <v>0.77957997338470042</v>
+      </c>
+      <c r="K98">
+        <v>2.6774193548387091E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
       <c r="I99">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J99">
+        <v>0.7772447380689459</v>
+      </c>
+      <c r="K99">
+        <v>2.6808510638297881E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H100">
         <v>9.5</v>
       </c>
       <c r="I100">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J100">
+        <v>0.77491649796108097</v>
+      </c>
+      <c r="K100">
+        <v>2.6842105263157889E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H101">
         <v>9.6</v>
       </c>
       <c r="I101">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J101">
+        <v>0.77259523210692804</v>
+      </c>
+      <c r="K101">
+        <v>2.6875000000000003E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
       <c r="I102">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J102">
+        <v>0.77028091961507894</v>
+      </c>
+      <c r="K102">
+        <v>2.6907216494845364E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
       <c r="I103">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J103">
+        <v>0.76797353965670601</v>
+      </c>
+      <c r="K103">
+        <v>2.6938775510204079E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
       <c r="I104">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J104">
+        <v>0.76567307146537378</v>
+      </c>
+      <c r="K104">
+        <v>2.6969696969696963E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H105">
         <v>10</v>
       </c>
       <c r="I105">
         <v>0.03</v>
+      </c>
+      <c r="J105">
+        <v>0.76337949433685315</v>
+      </c>
+      <c r="K105">
+        <v>2.7000000000000007E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All done. But no xll_bootstrap.chm file.
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\GR6250-2019\hw8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zfan2\source\repos\hw81\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AA1B6-3A3A-449C-8E4D-534C3B62A88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E794972-DFDF-4DAC-A886-AD4FD83A922C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,14 +55,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -2037,18 +2035,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E377A32-36B0-46CA-9461-D5EEF7A10455}">
   <dimension ref="B2:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2060,7 +2056,7 @@
         <v>-1887632</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2083,7 +2079,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2105,7 +2101,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2127,7 +2123,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2145,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2167,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2180,10 @@
       <c r="E10">
         <v>0.02</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,E10)</f>
+        <v>1405492</v>
+      </c>
       <c r="H10">
         <v>0.5</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2204,10 @@
       <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,E11)</f>
+        <v>1405866</v>
+      </c>
       <c r="H11">
         <v>0.6</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2228,10 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,E12)</f>
+        <v>1405602</v>
+      </c>
       <c r="H12">
         <v>0.7</v>
       </c>
@@ -2234,7 +2239,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2252,10 @@
       <c r="E13">
         <v>0.02</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,E13)</f>
+        <v>1405470</v>
+      </c>
       <c r="H13">
         <v>0.8</v>
       </c>
@@ -2255,7 +2263,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2276,10 @@
       <c r="E14">
         <v>0.03</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
+        <v>594</v>
+      </c>
       <c r="H14">
         <v>0.9</v>
       </c>
@@ -2276,7 +2287,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2300,10 @@
       <c r="E15">
         <v>0.03</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
+        <v>858</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
@@ -2297,7 +2311,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +2324,10 @@
       <c r="E16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
+        <v>616</v>
+      </c>
       <c r="H16">
         <v>1.1000000000000001</v>
       </c>
@@ -2318,7 +2335,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2348,10 @@
       <c r="E17">
         <v>0.03</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
+        <v>1254</v>
+      </c>
       <c r="H17">
         <v>1.2</v>
       </c>
@@ -2339,7 +2359,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H18">
         <v>1.3</v>
       </c>
@@ -2347,7 +2367,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H19">
         <v>1.4</v>
       </c>
@@ -2355,7 +2375,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H20">
         <v>1.5</v>
       </c>
@@ -2363,7 +2383,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>1.6</v>
       </c>
@@ -2371,7 +2391,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>1.7</v>
       </c>
@@ -2379,7 +2399,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1.8</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>1.9</v>
       </c>
@@ -2395,7 +2415,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H25">
         <v>2</v>
       </c>
@@ -2403,7 +2423,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H26">
         <v>2.1</v>
       </c>
@@ -2411,7 +2431,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
@@ -2419,7 +2439,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
@@ -2427,7 +2447,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H29">
         <v>2.4</v>
       </c>
@@ -2435,7 +2455,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H30">
         <v>2.5</v>
       </c>
@@ -2443,7 +2463,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H31">
         <v>2.6</v>
       </c>
@@ -2451,7 +2471,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H32">
         <v>2.7</v>
       </c>
@@ -2459,7 +2479,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33">
         <v>2.8</v>
       </c>
@@ -2467,7 +2487,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34">
         <v>2.9</v>
       </c>
@@ -2475,7 +2495,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35">
         <v>3</v>
       </c>
@@ -2483,7 +2503,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36">
         <v>3.1</v>
       </c>
@@ -2491,7 +2511,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37">
         <v>3.2</v>
       </c>
@@ -2499,7 +2519,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38">
         <v>3.3</v>
       </c>
@@ -2507,7 +2527,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39">
         <v>3.4</v>
       </c>
@@ -2515,7 +2535,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H40">
         <v>3.5</v>
       </c>
@@ -2523,7 +2543,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H41">
         <v>3.6</v>
       </c>
@@ -2531,7 +2551,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H42">
         <v>3.7</v>
       </c>
@@ -2539,7 +2559,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H43">
         <v>3.8</v>
       </c>
@@ -2547,7 +2567,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H44">
         <v>3.9</v>
       </c>
@@ -2555,7 +2575,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H45">
         <v>4</v>
       </c>
@@ -2563,7 +2583,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
@@ -2571,7 +2591,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H47">
         <v>4.2</v>
       </c>
@@ -2579,7 +2599,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H48">
         <v>4.3</v>
       </c>
@@ -2587,7 +2607,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
@@ -2595,7 +2615,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H50">
         <v>4.5</v>
       </c>
@@ -2603,7 +2623,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
@@ -2611,7 +2631,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H52">
         <v>4.7</v>
       </c>
@@ -2619,7 +2639,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H53">
         <v>4.8</v>
       </c>
@@ -2627,7 +2647,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
@@ -2635,7 +2655,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H55">
         <v>5</v>
       </c>
@@ -2643,7 +2663,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
@@ -2651,7 +2671,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H57">
         <v>5.2</v>
       </c>
@@ -2659,7 +2679,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H58">
         <v>5.3</v>
       </c>
@@ -2667,7 +2687,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H59">
         <v>5.4</v>
       </c>
@@ -2675,7 +2695,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H60">
         <v>5.5</v>
       </c>
@@ -2683,7 +2703,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H61">
         <v>5.6</v>
       </c>
@@ -2691,7 +2711,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H62">
         <v>5.7</v>
       </c>
@@ -2699,7 +2719,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H63">
         <v>5.8</v>
       </c>
@@ -2707,7 +2727,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H64">
         <v>5.9</v>
       </c>
@@ -2715,7 +2735,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H65">
         <v>6</v>
       </c>
@@ -2723,7 +2743,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H66">
         <v>6.1</v>
       </c>
@@ -2731,7 +2751,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H67">
         <v>6.2</v>
       </c>
@@ -2739,7 +2759,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H68">
         <v>6.3</v>
       </c>
@@ -2747,7 +2767,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H69">
         <v>6.4</v>
       </c>
@@ -2755,7 +2775,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H70">
         <v>6.5</v>
       </c>
@@ -2763,7 +2783,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H71">
         <v>6.6</v>
       </c>
@@ -2771,7 +2791,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H72">
         <v>6.7</v>
       </c>
@@ -2779,7 +2799,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H73">
         <v>6.8</v>
       </c>
@@ -2787,7 +2807,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H74">
         <v>6.9</v>
       </c>
@@ -2795,7 +2815,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H75">
         <v>7</v>
       </c>
@@ -2803,7 +2823,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H76">
         <v>7.1</v>
       </c>
@@ -2811,7 +2831,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H77">
         <v>7.2</v>
       </c>
@@ -2819,7 +2839,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H78">
         <v>7.3</v>
       </c>
@@ -2827,7 +2847,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H79">
         <v>7.4</v>
       </c>
@@ -2835,7 +2855,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H80">
         <v>7.5</v>
       </c>
@@ -2843,7 +2863,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H81">
         <v>7.6</v>
       </c>
@@ -2851,7 +2871,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82">
         <v>7.7</v>
       </c>
@@ -2859,7 +2879,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H83">
         <v>7.8</v>
       </c>
@@ -2867,7 +2887,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H84">
         <v>7.9</v>
       </c>
@@ -2875,7 +2895,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H85">
         <v>8</v>
       </c>
@@ -2883,7 +2903,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86">
         <v>8.1</v>
       </c>
@@ -2891,7 +2911,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
@@ -2899,7 +2919,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
@@ -2907,7 +2927,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H89">
         <v>8.4</v>
       </c>
@@ -2915,7 +2935,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H90">
         <v>8.5</v>
       </c>
@@ -2923,7 +2943,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H91">
         <v>8.6</v>
       </c>
@@ -2931,7 +2951,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
@@ -2939,7 +2959,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
@@ -2947,7 +2967,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H94">
         <v>8.9</v>
       </c>
@@ -2955,7 +2975,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H95">
         <v>9</v>
       </c>
@@ -2963,7 +2983,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H96">
         <v>9.1</v>
       </c>
@@ -2971,7 +2991,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
@@ -2979,7 +2999,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
@@ -2987,7 +3007,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
@@ -2995,7 +3015,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H100">
         <v>9.5</v>
       </c>
@@ -3003,7 +3023,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H101">
         <v>9.6</v>
       </c>
@@ -3011,7 +3031,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
@@ -3019,7 +3039,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
@@ -3027,7 +3047,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
@@ -3035,7 +3055,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H105">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
gw2376, Gaozhan Wang, HW8
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\GR6250-2019\hw8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangg\source\repos\hw8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AA1B6-3A3A-449C-8E4D-534C3B62A88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DDC364-B942-44CB-80B7-9A6BAB669163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
+    <workbookView xWindow="1140" yWindow="2430" windowWidth="23955" windowHeight="11295" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +43,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Create handles to fra's and swaps</t>
         </r>
@@ -57,14 +54,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -160,7 +157,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2038,17 +2035,20 @@
   <dimension ref="B2:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>-1887632</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2160,9 +2160,9 @@
       <c r="E9">
         <v>0.01</v>
       </c>
-      <c r="F9" cm="1">
-        <f t="array" ref="F9">_xll.INSTRUMENT.CASH_DEPOSIT(C9, E9)</f>
-        <v>276704</v>
+      <c r="F9">
+        <f>_xll.INSTRUMENT.CASH_DEPOSIT(C9, E9)</f>
+        <v>8</v>
       </c>
       <c r="H9">
         <v>0.4</v>
@@ -2171,7 +2171,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2184,10 @@
       <c r="E10">
         <v>0.02</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,A16)</f>
+        <v>-300</v>
+      </c>
       <c r="H10">
         <v>0.5</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2208,10 @@
       <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,A17)</f>
+        <v>-10441968</v>
+      </c>
       <c r="H11">
         <v>0.6</v>
       </c>
@@ -2213,7 +2219,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2232,10 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,A18)</f>
+        <v>-10441638</v>
+      </c>
       <c r="H12">
         <v>0.7</v>
       </c>
@@ -2234,7 +2243,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2256,10 @@
       <c r="E13">
         <v>0.02</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,A19)</f>
+        <v>-10442100</v>
+      </c>
       <c r="H13">
         <v>0.8</v>
       </c>
@@ -2255,7 +2267,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2280,10 @@
       <c r="E14">
         <v>0.03</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
+        <v>-10442298</v>
+      </c>
       <c r="H14">
         <v>0.9</v>
       </c>
@@ -2276,7 +2291,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2304,10 @@
       <c r="E15">
         <v>0.03</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
+        <v>-10441660</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
@@ -2297,7 +2315,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +2328,10 @@
       <c r="E16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
+        <v>-10442188</v>
+      </c>
       <c r="H16">
         <v>1.1000000000000001</v>
       </c>
@@ -2318,7 +2339,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2352,10 @@
       <c r="E17">
         <v>0.03</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
+        <v>-10441924</v>
+      </c>
       <c r="H17">
         <v>1.2</v>
       </c>
@@ -2339,7 +2363,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H18">
         <v>1.3</v>
       </c>
@@ -2347,7 +2371,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H19">
         <v>1.4</v>
       </c>
@@ -2355,7 +2379,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H20">
         <v>1.5</v>
       </c>
@@ -2363,7 +2387,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>1.6</v>
       </c>
@@ -2371,7 +2395,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>1.7</v>
       </c>
@@ -2379,7 +2403,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1.8</v>
       </c>
@@ -2387,7 +2411,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>1.9</v>
       </c>
@@ -2395,7 +2419,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H25">
         <v>2</v>
       </c>
@@ -2403,7 +2427,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H26">
         <v>2.1</v>
       </c>
@@ -2411,7 +2435,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
@@ -2419,7 +2443,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
@@ -2427,7 +2451,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H29">
         <v>2.4</v>
       </c>
@@ -2435,7 +2459,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H30">
         <v>2.5</v>
       </c>
@@ -2443,7 +2467,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H31">
         <v>2.6</v>
       </c>
@@ -2451,7 +2475,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H32">
         <v>2.7</v>
       </c>
@@ -2459,7 +2483,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33">
         <v>2.8</v>
       </c>
@@ -2467,7 +2491,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34">
         <v>2.9</v>
       </c>
@@ -2475,7 +2499,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35">
         <v>3</v>
       </c>
@@ -2483,7 +2507,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36">
         <v>3.1</v>
       </c>
@@ -2491,7 +2515,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37">
         <v>3.2</v>
       </c>
@@ -2499,7 +2523,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38">
         <v>3.3</v>
       </c>
@@ -2507,7 +2531,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39">
         <v>3.4</v>
       </c>
@@ -2515,7 +2539,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H40">
         <v>3.5</v>
       </c>
@@ -2523,7 +2547,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H41">
         <v>3.6</v>
       </c>
@@ -2531,7 +2555,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H42">
         <v>3.7</v>
       </c>
@@ -2539,7 +2563,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H43">
         <v>3.8</v>
       </c>
@@ -2547,7 +2571,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H44">
         <v>3.9</v>
       </c>
@@ -2555,7 +2579,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H45">
         <v>4</v>
       </c>
@@ -2563,7 +2587,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
@@ -2571,7 +2595,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H47">
         <v>4.2</v>
       </c>
@@ -2579,7 +2603,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H48">
         <v>4.3</v>
       </c>
@@ -2587,7 +2611,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
@@ -2595,7 +2619,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H50">
         <v>4.5</v>
       </c>
@@ -2603,7 +2627,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
@@ -2611,7 +2635,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H52">
         <v>4.7</v>
       </c>
@@ -2619,7 +2643,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H53">
         <v>4.8</v>
       </c>
@@ -2627,7 +2651,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
@@ -2635,7 +2659,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H55">
         <v>5</v>
       </c>
@@ -2643,7 +2667,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
@@ -2651,7 +2675,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H57">
         <v>5.2</v>
       </c>
@@ -2659,7 +2683,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H58">
         <v>5.3</v>
       </c>
@@ -2667,7 +2691,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H59">
         <v>5.4</v>
       </c>
@@ -2675,7 +2699,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H60">
         <v>5.5</v>
       </c>
@@ -2683,7 +2707,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H61">
         <v>5.6</v>
       </c>
@@ -2691,7 +2715,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H62">
         <v>5.7</v>
       </c>
@@ -2699,7 +2723,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H63">
         <v>5.8</v>
       </c>
@@ -2707,7 +2731,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H64">
         <v>5.9</v>
       </c>
@@ -2715,7 +2739,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H65">
         <v>6</v>
       </c>
@@ -2723,7 +2747,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H66">
         <v>6.1</v>
       </c>
@@ -2731,7 +2755,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H67">
         <v>6.2</v>
       </c>
@@ -2739,7 +2763,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H68">
         <v>6.3</v>
       </c>
@@ -2747,7 +2771,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H69">
         <v>6.4</v>
       </c>
@@ -2755,7 +2779,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H70">
         <v>6.5</v>
       </c>
@@ -2763,7 +2787,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H71">
         <v>6.6</v>
       </c>
@@ -2771,7 +2795,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H72">
         <v>6.7</v>
       </c>
@@ -2779,7 +2803,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H73">
         <v>6.8</v>
       </c>
@@ -2787,7 +2811,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H74">
         <v>6.9</v>
       </c>
@@ -2795,7 +2819,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H75">
         <v>7</v>
       </c>
@@ -2803,7 +2827,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H76">
         <v>7.1</v>
       </c>
@@ -2811,7 +2835,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H77">
         <v>7.2</v>
       </c>
@@ -2819,7 +2843,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H78">
         <v>7.3</v>
       </c>
@@ -2827,7 +2851,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H79">
         <v>7.4</v>
       </c>
@@ -2835,7 +2859,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H80">
         <v>7.5</v>
       </c>
@@ -2843,7 +2867,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H81">
         <v>7.6</v>
       </c>
@@ -2851,7 +2875,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82">
         <v>7.7</v>
       </c>
@@ -2859,7 +2883,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H83">
         <v>7.8</v>
       </c>
@@ -2867,7 +2891,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H84">
         <v>7.9</v>
       </c>
@@ -2875,7 +2899,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H85">
         <v>8</v>
       </c>
@@ -2883,7 +2907,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86">
         <v>8.1</v>
       </c>
@@ -2891,7 +2915,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
@@ -2899,7 +2923,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
@@ -2907,7 +2931,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H89">
         <v>8.4</v>
       </c>
@@ -2915,7 +2939,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H90">
         <v>8.5</v>
       </c>
@@ -2923,7 +2947,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H91">
         <v>8.6</v>
       </c>
@@ -2931,7 +2955,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
@@ -2939,7 +2963,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
@@ -2947,7 +2971,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H94">
         <v>8.9</v>
       </c>
@@ -2955,7 +2979,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H95">
         <v>9</v>
       </c>
@@ -2963,7 +2987,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H96">
         <v>9.1</v>
       </c>
@@ -2971,7 +2995,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
@@ -2979,7 +3003,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
@@ -2987,7 +3011,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
@@ -2995,7 +3019,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H100">
         <v>9.5</v>
       </c>
@@ -3003,7 +3027,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H101">
         <v>9.6</v>
       </c>
@@ -3011,7 +3035,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
@@ -3019,7 +3043,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
@@ -3027,7 +3051,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
@@ -3035,7 +3059,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H105">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Gihyen Eom - ge2247 Assignment 8
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\GR6250-2019\hw8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\source\repos\hw8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AA1B6-3A3A-449C-8E4D-534C3B62A88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA48288-4E6B-421F-A843-B673E3ED252A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +43,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Create handles to fra's and swaps</t>
         </r>
@@ -57,14 +54,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -160,7 +157,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2038,17 +2035,17 @@
   <dimension ref="B2:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2057,10 +2054,10 @@
       </c>
       <c r="I4" cm="1">
         <f t="array" ref="I4">_xll.PWFLAT.FORWARD(C5:C17,E5:E17)</f>
-        <v>-1887632</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+        <v>-3389</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2073,7 +2070,7 @@
       </c>
       <c r="F5" cm="1">
         <f t="array" ref="F5">_xll.INSTRUMENT.CASH_DEPOSIT(C5, E5)</f>
-        <v>276992</v>
+        <v>-146</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2083,7 +2080,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2096,7 +2093,7 @@
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">_xll.INSTRUMENT.CASH_DEPOSIT(C6, E6)</f>
-        <v>276680</v>
+        <v>-256</v>
       </c>
       <c r="H6">
         <v>0.1</v>
@@ -2105,7 +2102,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2118,7 +2115,7 @@
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">_xll.INSTRUMENT.CASH_DEPOSIT(C7, E7)</f>
-        <v>276776</v>
+        <v>558</v>
       </c>
       <c r="H7">
         <v>0.2</v>
@@ -2127,7 +2124,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2140,7 +2137,7 @@
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.INSTRUMENT.CASH_DEPOSIT(C8, E8)</f>
-        <v>276728</v>
+        <v>-366</v>
       </c>
       <c r="H8">
         <v>0.3</v>
@@ -2149,7 +2146,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2162,7 +2159,7 @@
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">_xll.INSTRUMENT.CASH_DEPOSIT(C9, E9)</f>
-        <v>276704</v>
+        <v>316</v>
       </c>
       <c r="H9">
         <v>0.4</v>
@@ -2171,7 +2168,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2181,10 @@
       <c r="E10">
         <v>0.02</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,E10)</f>
+        <v>448</v>
+      </c>
       <c r="H10">
         <v>0.5</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2205,10 @@
       <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,E11)</f>
+        <v>580</v>
+      </c>
       <c r="H11">
         <v>0.6</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2229,10 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,E12)</f>
+        <v>118</v>
+      </c>
       <c r="H12">
         <v>0.7</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2253,10 @@
       <c r="E13">
         <v>0.02</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,E13)</f>
+        <v>-608</v>
+      </c>
       <c r="H13">
         <v>0.8</v>
       </c>
@@ -2255,7 +2264,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2277,10 @@
       <c r="E14">
         <v>0.03</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
+        <v>-14</v>
+      </c>
       <c r="H14">
         <v>0.9</v>
       </c>
@@ -2276,7 +2288,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2301,10 @@
       <c r="E15">
         <v>0.03</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
+        <v>30</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
@@ -2297,7 +2312,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +2325,10 @@
       <c r="E16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
+        <v>-564</v>
+      </c>
       <c r="H16">
         <v>1.1000000000000001</v>
       </c>
@@ -2318,7 +2336,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2349,10 @@
       <c r="E17">
         <v>0.03</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
+        <v>-498</v>
+      </c>
       <c r="H17">
         <v>1.2</v>
       </c>
@@ -2339,7 +2360,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>1.3</v>
       </c>
@@ -2347,7 +2368,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>1.4</v>
       </c>
@@ -2355,7 +2376,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>1.5</v>
       </c>
@@ -2363,7 +2384,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>1.6</v>
       </c>
@@ -2371,7 +2392,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H22">
         <v>1.7</v>
       </c>
@@ -2379,7 +2400,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H23">
         <v>1.8</v>
       </c>
@@ -2387,7 +2408,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>1.9</v>
       </c>
@@ -2395,7 +2416,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H25">
         <v>2</v>
       </c>
@@ -2403,7 +2424,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H26">
         <v>2.1</v>
       </c>
@@ -2411,7 +2432,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
@@ -2419,7 +2440,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
@@ -2427,7 +2448,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H29">
         <v>2.4</v>
       </c>
@@ -2435,7 +2456,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>2.5</v>
       </c>
@@ -2443,7 +2464,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H31">
         <v>2.6</v>
       </c>
@@ -2451,7 +2472,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H32">
         <v>2.7</v>
       </c>
@@ -2459,7 +2480,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33">
         <v>2.8</v>
       </c>
@@ -2467,7 +2488,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34">
         <v>2.9</v>
       </c>
@@ -2475,7 +2496,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35">
         <v>3</v>
       </c>
@@ -2483,7 +2504,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36">
         <v>3.1</v>
       </c>
@@ -2491,7 +2512,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37">
         <v>3.2</v>
       </c>
@@ -2499,7 +2520,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38">
         <v>3.3</v>
       </c>
@@ -2507,7 +2528,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39">
         <v>3.4</v>
       </c>
@@ -2515,7 +2536,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H40">
         <v>3.5</v>
       </c>
@@ -2523,7 +2544,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H41">
         <v>3.6</v>
       </c>
@@ -2531,7 +2552,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H42">
         <v>3.7</v>
       </c>
@@ -2539,7 +2560,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H43">
         <v>3.8</v>
       </c>
@@ -2547,7 +2568,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H44">
         <v>3.9</v>
       </c>
@@ -2555,7 +2576,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H45">
         <v>4</v>
       </c>
@@ -2563,7 +2584,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
@@ -2571,7 +2592,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H47">
         <v>4.2</v>
       </c>
@@ -2579,7 +2600,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H48">
         <v>4.3</v>
       </c>
@@ -2587,7 +2608,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
@@ -2595,7 +2616,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H50">
         <v>4.5</v>
       </c>
@@ -2603,7 +2624,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
@@ -2611,7 +2632,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H52">
         <v>4.7</v>
       </c>
@@ -2619,7 +2640,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H53">
         <v>4.8</v>
       </c>
@@ -2627,7 +2648,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
@@ -2635,7 +2656,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H55">
         <v>5</v>
       </c>
@@ -2643,7 +2664,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
@@ -2651,7 +2672,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H57">
         <v>5.2</v>
       </c>
@@ -2659,7 +2680,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H58">
         <v>5.3</v>
       </c>
@@ -2667,7 +2688,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H59">
         <v>5.4</v>
       </c>
@@ -2675,7 +2696,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H60">
         <v>5.5</v>
       </c>
@@ -2683,7 +2704,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H61">
         <v>5.6</v>
       </c>
@@ -2691,7 +2712,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H62">
         <v>5.7</v>
       </c>
@@ -2699,7 +2720,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H63">
         <v>5.8</v>
       </c>
@@ -2707,7 +2728,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H64">
         <v>5.9</v>
       </c>
@@ -2715,7 +2736,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H65">
         <v>6</v>
       </c>
@@ -2723,7 +2744,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H66">
         <v>6.1</v>
       </c>
@@ -2731,7 +2752,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H67">
         <v>6.2</v>
       </c>
@@ -2739,7 +2760,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H68">
         <v>6.3</v>
       </c>
@@ -2747,7 +2768,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H69">
         <v>6.4</v>
       </c>
@@ -2755,7 +2776,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H70">
         <v>6.5</v>
       </c>
@@ -2763,7 +2784,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H71">
         <v>6.6</v>
       </c>
@@ -2771,7 +2792,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H72">
         <v>6.7</v>
       </c>
@@ -2779,7 +2800,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H73">
         <v>6.8</v>
       </c>
@@ -2787,7 +2808,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H74">
         <v>6.9</v>
       </c>
@@ -2795,7 +2816,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H75">
         <v>7</v>
       </c>
@@ -2803,7 +2824,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H76">
         <v>7.1</v>
       </c>
@@ -2811,7 +2832,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H77">
         <v>7.2</v>
       </c>
@@ -2819,7 +2840,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H78">
         <v>7.3</v>
       </c>
@@ -2827,7 +2848,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H79">
         <v>7.4</v>
       </c>
@@ -2835,7 +2856,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H80">
         <v>7.5</v>
       </c>
@@ -2843,7 +2864,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H81">
         <v>7.6</v>
       </c>
@@ -2851,7 +2872,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H82">
         <v>7.7</v>
       </c>
@@ -2859,7 +2880,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H83">
         <v>7.8</v>
       </c>
@@ -2867,7 +2888,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H84">
         <v>7.9</v>
       </c>
@@ -2875,7 +2896,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H85">
         <v>8</v>
       </c>
@@ -2883,7 +2904,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H86">
         <v>8.1</v>
       </c>
@@ -2891,7 +2912,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
@@ -2899,7 +2920,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
@@ -2907,7 +2928,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H89">
         <v>8.4</v>
       </c>
@@ -2915,7 +2936,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H90">
         <v>8.5</v>
       </c>
@@ -2923,7 +2944,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H91">
         <v>8.6</v>
       </c>
@@ -2931,7 +2952,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
@@ -2939,7 +2960,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
@@ -2947,7 +2968,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H94">
         <v>8.9</v>
       </c>
@@ -2955,7 +2976,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H95">
         <v>9</v>
       </c>
@@ -2963,7 +2984,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H96">
         <v>9.1</v>
       </c>
@@ -2971,7 +2992,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
@@ -2979,7 +3000,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
@@ -2987,7 +3008,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
@@ -2995,7 +3016,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H100">
         <v>9.5</v>
       </c>
@@ -3003,7 +3024,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H101">
         <v>9.6</v>
       </c>
@@ -3011,7 +3032,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
@@ -3019,7 +3040,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
@@ -3027,7 +3048,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
@@ -3035,7 +3056,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H105">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
hw 8  Ruiqing Liu rl3107
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\GR6250-2019\hw8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zfan2\source\repos\hw81\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AA1B6-3A3A-449C-8E4D-534C3B62A88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE5AEF4-CD77-4A80-A3AB-EFB75F0573A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,14 +55,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -2037,18 +2035,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E377A32-36B0-46CA-9461-D5EEF7A10455}">
   <dimension ref="B2:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2060,7 +2056,7 @@
         <v>-1887632</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2083,7 +2079,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2105,7 +2101,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2127,7 +2123,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2145,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2167,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2180,10 @@
       <c r="E10">
         <v>0.02</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,E10)</f>
+        <v>1405492</v>
+      </c>
       <c r="H10">
         <v>0.5</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2204,10 @@
       <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,E11)</f>
+        <v>1405866</v>
+      </c>
       <c r="H11">
         <v>0.6</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2228,10 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,E12)</f>
+        <v>1405602</v>
+      </c>
       <c r="H12">
         <v>0.7</v>
       </c>
@@ -2234,7 +2239,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2252,10 @@
       <c r="E13">
         <v>0.02</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,E13)</f>
+        <v>1405470</v>
+      </c>
       <c r="H13">
         <v>0.8</v>
       </c>
@@ -2255,7 +2263,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2276,10 @@
       <c r="E14">
         <v>0.03</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
+        <v>594</v>
+      </c>
       <c r="H14">
         <v>0.9</v>
       </c>
@@ -2276,7 +2287,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2300,10 @@
       <c r="E15">
         <v>0.03</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
+        <v>858</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
@@ -2297,7 +2311,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +2324,10 @@
       <c r="E16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
+        <v>616</v>
+      </c>
       <c r="H16">
         <v>1.1000000000000001</v>
       </c>
@@ -2318,7 +2335,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2348,10 @@
       <c r="E17">
         <v>0.03</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
+        <v>1254</v>
+      </c>
       <c r="H17">
         <v>1.2</v>
       </c>
@@ -2339,7 +2359,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H18">
         <v>1.3</v>
       </c>
@@ -2347,7 +2367,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H19">
         <v>1.4</v>
       </c>
@@ -2355,7 +2375,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H20">
         <v>1.5</v>
       </c>
@@ -2363,7 +2383,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>1.6</v>
       </c>
@@ -2371,7 +2391,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>1.7</v>
       </c>
@@ -2379,7 +2399,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1.8</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>1.9</v>
       </c>
@@ -2395,7 +2415,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H25">
         <v>2</v>
       </c>
@@ -2403,7 +2423,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H26">
         <v>2.1</v>
       </c>
@@ -2411,7 +2431,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
@@ -2419,7 +2439,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
@@ -2427,7 +2447,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H29">
         <v>2.4</v>
       </c>
@@ -2435,7 +2455,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H30">
         <v>2.5</v>
       </c>
@@ -2443,7 +2463,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H31">
         <v>2.6</v>
       </c>
@@ -2451,7 +2471,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H32">
         <v>2.7</v>
       </c>
@@ -2459,7 +2479,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33">
         <v>2.8</v>
       </c>
@@ -2467,7 +2487,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34">
         <v>2.9</v>
       </c>
@@ -2475,7 +2495,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35">
         <v>3</v>
       </c>
@@ -2483,7 +2503,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36">
         <v>3.1</v>
       </c>
@@ -2491,7 +2511,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37">
         <v>3.2</v>
       </c>
@@ -2499,7 +2519,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38">
         <v>3.3</v>
       </c>
@@ -2507,7 +2527,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39">
         <v>3.4</v>
       </c>
@@ -2515,7 +2535,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H40">
         <v>3.5</v>
       </c>
@@ -2523,7 +2543,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H41">
         <v>3.6</v>
       </c>
@@ -2531,7 +2551,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H42">
         <v>3.7</v>
       </c>
@@ -2539,7 +2559,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H43">
         <v>3.8</v>
       </c>
@@ -2547,7 +2567,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H44">
         <v>3.9</v>
       </c>
@@ -2555,7 +2575,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H45">
         <v>4</v>
       </c>
@@ -2563,7 +2583,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
@@ -2571,7 +2591,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H47">
         <v>4.2</v>
       </c>
@@ -2579,7 +2599,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H48">
         <v>4.3</v>
       </c>
@@ -2587,7 +2607,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
@@ -2595,7 +2615,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H50">
         <v>4.5</v>
       </c>
@@ -2603,7 +2623,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
@@ -2611,7 +2631,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H52">
         <v>4.7</v>
       </c>
@@ -2619,7 +2639,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H53">
         <v>4.8</v>
       </c>
@@ -2627,7 +2647,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
@@ -2635,7 +2655,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H55">
         <v>5</v>
       </c>
@@ -2643,7 +2663,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
@@ -2651,7 +2671,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H57">
         <v>5.2</v>
       </c>
@@ -2659,7 +2679,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H58">
         <v>5.3</v>
       </c>
@@ -2667,7 +2687,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H59">
         <v>5.4</v>
       </c>
@@ -2675,7 +2695,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H60">
         <v>5.5</v>
       </c>
@@ -2683,7 +2703,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H61">
         <v>5.6</v>
       </c>
@@ -2691,7 +2711,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H62">
         <v>5.7</v>
       </c>
@@ -2699,7 +2719,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H63">
         <v>5.8</v>
       </c>
@@ -2707,7 +2727,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H64">
         <v>5.9</v>
       </c>
@@ -2715,7 +2735,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H65">
         <v>6</v>
       </c>
@@ -2723,7 +2743,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H66">
         <v>6.1</v>
       </c>
@@ -2731,7 +2751,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H67">
         <v>6.2</v>
       </c>
@@ -2739,7 +2759,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H68">
         <v>6.3</v>
       </c>
@@ -2747,7 +2767,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H69">
         <v>6.4</v>
       </c>
@@ -2755,7 +2775,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H70">
         <v>6.5</v>
       </c>
@@ -2763,7 +2783,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H71">
         <v>6.6</v>
       </c>
@@ -2771,7 +2791,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H72">
         <v>6.7</v>
       </c>
@@ -2779,7 +2799,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H73">
         <v>6.8</v>
       </c>
@@ -2787,7 +2807,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H74">
         <v>6.9</v>
       </c>
@@ -2795,7 +2815,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H75">
         <v>7</v>
       </c>
@@ -2803,7 +2823,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H76">
         <v>7.1</v>
       </c>
@@ -2811,7 +2831,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H77">
         <v>7.2</v>
       </c>
@@ -2819,7 +2839,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H78">
         <v>7.3</v>
       </c>
@@ -2827,7 +2847,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H79">
         <v>7.4</v>
       </c>
@@ -2835,7 +2855,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H80">
         <v>7.5</v>
       </c>
@@ -2843,7 +2863,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H81">
         <v>7.6</v>
       </c>
@@ -2851,7 +2871,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82">
         <v>7.7</v>
       </c>
@@ -2859,7 +2879,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H83">
         <v>7.8</v>
       </c>
@@ -2867,7 +2887,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H84">
         <v>7.9</v>
       </c>
@@ -2875,7 +2895,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H85">
         <v>8</v>
       </c>
@@ -2883,7 +2903,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86">
         <v>8.1</v>
       </c>
@@ -2891,7 +2911,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
@@ -2899,7 +2919,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
@@ -2907,7 +2927,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H89">
         <v>8.4</v>
       </c>
@@ -2915,7 +2935,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H90">
         <v>8.5</v>
       </c>
@@ -2923,7 +2943,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H91">
         <v>8.6</v>
       </c>
@@ -2931,7 +2951,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
@@ -2939,7 +2959,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
@@ -2947,7 +2967,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H94">
         <v>8.9</v>
       </c>
@@ -2955,7 +2975,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H95">
         <v>9</v>
       </c>
@@ -2963,7 +2983,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H96">
         <v>9.1</v>
       </c>
@@ -2971,7 +2991,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
@@ -2979,7 +2999,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
@@ -2987,7 +3007,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
@@ -2995,7 +3015,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H100">
         <v>9.5</v>
       </c>
@@ -3003,7 +3023,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H101">
         <v>9.6</v>
       </c>
@@ -3011,7 +3031,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
@@ -3019,7 +3039,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
@@ -3027,7 +3047,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
@@ -3035,7 +3055,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H105">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Revert "hw 8  Ruiqing Liu rl3107"
This reverts commit e7445e91d2f9b8f13a2da83475518e34fec525dd.
</commit_message>
<xml_diff>
--- a/hw8.xlsx
+++ b/hw8.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zfan2\source\repos\hw81\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\GR6250-2019\hw8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE5AEF4-CD77-4A80-A3AB-EFB75F0573A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AA1B6-3A3A-449C-8E4D-534C3B62A88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{FCFFA66E-F09B-406E-84E0-990A9ACED936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -55,14 +57,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -2035,16 +2037,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E377A32-36B0-46CA-9461-D5EEF7A10455}">
   <dimension ref="B2:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>-1887632</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2101,7 +2105,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2145,7 +2149,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2167,7 +2171,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2180,10 +2184,7 @@
       <c r="E10">
         <v>0.02</v>
       </c>
-      <c r="F10" s="4">
-        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C10,D10,E10)</f>
-        <v>1405492</v>
-      </c>
+      <c r="F10" s="4"/>
       <c r="H10">
         <v>0.5</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2204,10 +2205,7 @@
       <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="F11" s="4">
-        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C11,D11,E11)</f>
-        <v>1405866</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="H11">
         <v>0.6</v>
       </c>
@@ -2215,7 +2213,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2228,10 +2226,7 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="4">
-        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C12,D12,E12)</f>
-        <v>1405602</v>
-      </c>
+      <c r="F12" s="4"/>
       <c r="H12">
         <v>0.7</v>
       </c>
@@ -2239,7 +2234,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2252,10 +2247,7 @@
       <c r="E13">
         <v>0.02</v>
       </c>
-      <c r="F13" s="4">
-        <f>_xll.INSTRUMENT.FORWARD_RATE_AGREEMENT(C13,D13,E13)</f>
-        <v>1405470</v>
-      </c>
+      <c r="F13" s="4"/>
       <c r="H13">
         <v>0.8</v>
       </c>
@@ -2263,7 +2255,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2276,10 +2268,7 @@
       <c r="E14">
         <v>0.03</v>
       </c>
-      <c r="F14" s="4">
-        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C14,D14,E14)</f>
-        <v>594</v>
-      </c>
+      <c r="F14" s="4"/>
       <c r="H14">
         <v>0.9</v>
       </c>
@@ -2287,7 +2276,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2300,10 +2289,7 @@
       <c r="E15">
         <v>0.03</v>
       </c>
-      <c r="F15" s="4">
-        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C15,D15,E15)</f>
-        <v>858</v>
-      </c>
+      <c r="F15" s="4"/>
       <c r="H15">
         <v>1</v>
       </c>
@@ -2311,7 +2297,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2324,10 +2310,7 @@
       <c r="E16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="4">
-        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C16,D16,E16)</f>
-        <v>616</v>
-      </c>
+      <c r="F16" s="4"/>
       <c r="H16">
         <v>1.1000000000000001</v>
       </c>
@@ -2335,7 +2318,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2348,10 +2331,7 @@
       <c r="E17">
         <v>0.03</v>
       </c>
-      <c r="F17" s="4">
-        <f>_xll.INSTRUMENT.INTEREST_RATE_SWAP(C17,D17,E17)</f>
-        <v>1254</v>
-      </c>
+      <c r="F17" s="4"/>
       <c r="H17">
         <v>1.2</v>
       </c>
@@ -2359,7 +2339,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H18">
         <v>1.3</v>
       </c>
@@ -2367,7 +2347,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H19">
         <v>1.4</v>
       </c>
@@ -2375,7 +2355,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H20">
         <v>1.5</v>
       </c>
@@ -2383,7 +2363,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H21">
         <v>1.6</v>
       </c>
@@ -2391,7 +2371,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H22">
         <v>1.7</v>
       </c>
@@ -2399,7 +2379,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H23">
         <v>1.8</v>
       </c>
@@ -2407,7 +2387,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H24">
         <v>1.9</v>
       </c>
@@ -2415,7 +2395,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H25">
         <v>2</v>
       </c>
@@ -2423,7 +2403,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H26">
         <v>2.1</v>
       </c>
@@ -2431,7 +2411,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H27">
         <v>2.2000000000000002</v>
       </c>
@@ -2439,7 +2419,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H28">
         <v>2.2999999999999998</v>
       </c>
@@ -2447,7 +2427,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H29">
         <v>2.4</v>
       </c>
@@ -2455,7 +2435,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H30">
         <v>2.5</v>
       </c>
@@ -2463,7 +2443,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H31">
         <v>2.6</v>
       </c>
@@ -2471,7 +2451,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
       <c r="H32">
         <v>2.7</v>
       </c>
@@ -2479,7 +2459,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H33">
         <v>2.8</v>
       </c>
@@ -2487,7 +2467,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H34">
         <v>2.9</v>
       </c>
@@ -2495,7 +2475,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H35">
         <v>3</v>
       </c>
@@ -2503,7 +2483,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H36">
         <v>3.1</v>
       </c>
@@ -2511,7 +2491,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H37">
         <v>3.2</v>
       </c>
@@ -2519,7 +2499,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H38">
         <v>3.3</v>
       </c>
@@ -2527,7 +2507,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H39">
         <v>3.4</v>
       </c>
@@ -2535,7 +2515,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H40">
         <v>3.5</v>
       </c>
@@ -2543,7 +2523,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H41">
         <v>3.6</v>
       </c>
@@ -2551,7 +2531,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H42">
         <v>3.7</v>
       </c>
@@ -2559,7 +2539,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H43">
         <v>3.8</v>
       </c>
@@ -2567,7 +2547,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H44">
         <v>3.9</v>
       </c>
@@ -2575,7 +2555,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H45">
         <v>4</v>
       </c>
@@ -2583,7 +2563,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H46">
         <v>4.0999999999999996</v>
       </c>
@@ -2591,7 +2571,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H47">
         <v>4.2</v>
       </c>
@@ -2599,7 +2579,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H48">
         <v>4.3</v>
       </c>
@@ -2607,7 +2587,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H49">
         <v>4.4000000000000004</v>
       </c>
@@ -2615,7 +2595,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H50">
         <v>4.5</v>
       </c>
@@ -2623,7 +2603,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H51">
         <v>4.5999999999999996</v>
       </c>
@@ -2631,7 +2611,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H52">
         <v>4.7</v>
       </c>
@@ -2639,7 +2619,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H53">
         <v>4.8</v>
       </c>
@@ -2647,7 +2627,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H54">
         <v>4.9000000000000004</v>
       </c>
@@ -2655,7 +2635,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H55">
         <v>5</v>
       </c>
@@ -2663,7 +2643,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H56">
         <v>5.0999999999999996</v>
       </c>
@@ -2671,7 +2651,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H57">
         <v>5.2</v>
       </c>
@@ -2679,7 +2659,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H58">
         <v>5.3</v>
       </c>
@@ -2687,7 +2667,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H59">
         <v>5.4</v>
       </c>
@@ -2695,7 +2675,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H60">
         <v>5.5</v>
       </c>
@@ -2703,7 +2683,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H61">
         <v>5.6</v>
       </c>
@@ -2711,7 +2691,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H62">
         <v>5.7</v>
       </c>
@@ -2719,7 +2699,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H63">
         <v>5.8</v>
       </c>
@@ -2727,7 +2707,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H64">
         <v>5.9</v>
       </c>
@@ -2735,7 +2715,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H65">
         <v>6</v>
       </c>
@@ -2743,7 +2723,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H66">
         <v>6.1</v>
       </c>
@@ -2751,7 +2731,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H67">
         <v>6.2</v>
       </c>
@@ -2759,7 +2739,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H68">
         <v>6.3</v>
       </c>
@@ -2767,7 +2747,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H69">
         <v>6.4</v>
       </c>
@@ -2775,7 +2755,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H70">
         <v>6.5</v>
       </c>
@@ -2783,7 +2763,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H71">
         <v>6.6</v>
       </c>
@@ -2791,7 +2771,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H72">
         <v>6.7</v>
       </c>
@@ -2799,7 +2779,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H73">
         <v>6.8</v>
       </c>
@@ -2807,7 +2787,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H74">
         <v>6.9</v>
       </c>
@@ -2815,7 +2795,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H75">
         <v>7</v>
       </c>
@@ -2823,7 +2803,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H76">
         <v>7.1</v>
       </c>
@@ -2831,7 +2811,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H77">
         <v>7.2</v>
       </c>
@@ -2839,7 +2819,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H78">
         <v>7.3</v>
       </c>
@@ -2847,7 +2827,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H79">
         <v>7.4</v>
       </c>
@@ -2855,7 +2835,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H80">
         <v>7.5</v>
       </c>
@@ -2863,7 +2843,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H81">
         <v>7.6</v>
       </c>
@@ -2871,7 +2851,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H82">
         <v>7.7</v>
       </c>
@@ -2879,7 +2859,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H83">
         <v>7.8</v>
       </c>
@@ -2887,7 +2867,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H84">
         <v>7.9</v>
       </c>
@@ -2895,7 +2875,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H85">
         <v>8</v>
       </c>
@@ -2903,7 +2883,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H86">
         <v>8.1</v>
       </c>
@@ -2911,7 +2891,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H87">
         <v>8.1999999999999993</v>
       </c>
@@ -2919,7 +2899,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H88">
         <v>8.3000000000000007</v>
       </c>
@@ -2927,7 +2907,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H89">
         <v>8.4</v>
       </c>
@@ -2935,7 +2915,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H90">
         <v>8.5</v>
       </c>
@@ -2943,7 +2923,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H91">
         <v>8.6</v>
       </c>
@@ -2951,7 +2931,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H92">
         <v>8.6999999999999993</v>
       </c>
@@ -2959,7 +2939,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H93">
         <v>8.8000000000000007</v>
       </c>
@@ -2967,7 +2947,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H94">
         <v>8.9</v>
       </c>
@@ -2975,7 +2955,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H95">
         <v>9</v>
       </c>
@@ -2983,7 +2963,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H96">
         <v>9.1</v>
       </c>
@@ -2991,7 +2971,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H97">
         <v>9.1999999999999993</v>
       </c>
@@ -2999,7 +2979,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H98">
         <v>9.3000000000000007</v>
       </c>
@@ -3007,7 +2987,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H99">
         <v>9.4000000000000092</v>
       </c>
@@ -3015,7 +2995,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H100">
         <v>9.5</v>
       </c>
@@ -3023,7 +3003,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H101">
         <v>9.6</v>
       </c>
@@ -3031,7 +3011,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H102">
         <v>9.7000000000000099</v>
       </c>
@@ -3039,7 +3019,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H103">
         <v>9.8000000000000096</v>
       </c>
@@ -3047,7 +3027,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H104">
         <v>9.9000000000000092</v>
       </c>
@@ -3055,7 +3035,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H105">
         <v>10</v>
       </c>

</xml_diff>